<commit_message>
added numbers, figure refs
</commit_message>
<xml_diff>
--- a/Milestone_3/Usability_Results.xlsx
+++ b/Milestone_3/Usability_Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="960" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="1740" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Timestamp</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Adding Classes to Wishlist/Planner</t>
+  </si>
+  <si>
+    <t>TOTAL MOS</t>
+  </si>
+  <si>
+    <t>TOTAL NEW</t>
+  </si>
+  <si>
+    <t>DIF</t>
   </si>
 </sst>
 </file>
@@ -3390,15 +3399,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>1272559</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>83024</xdr:rowOff>
+      <xdr:colOff>1386291</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>783609</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>139132</xdr:rowOff>
+      <xdr:colOff>897341</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3745,8 +3754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4674,6 +4683,13 @@
       <c r="AA12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="AB12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC12" s="4">
+        <f>SUM(AC11,AE11,AG11)</f>
+        <v>1.4319444444444447</v>
+      </c>
     </row>
     <row r="13" spans="1:35" ht="17" x14ac:dyDescent="0.2">
       <c r="X13" s="2" t="s">
@@ -4688,7 +4704,13 @@
       <c r="AA13" s="5">
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="AC13" s="3"/>
+      <c r="AB13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC13" s="3">
+        <f>SUM(AD11+AF11+AH11)</f>
+        <v>0.5131944444444444</v>
+      </c>
     </row>
     <row r="14" spans="1:35" ht="17" x14ac:dyDescent="0.2">
       <c r="X14" s="2" t="s">
@@ -4702,6 +4724,13 @@
       </c>
       <c r="AA14" s="5">
         <v>2.6041666666666665E-3</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC14" s="2">
+        <f>AC13/AC12</f>
+        <v>0.35838991270611048</v>
       </c>
     </row>
     <row r="40" spans="19:26" x14ac:dyDescent="0.2">

</xml_diff>